<commit_message>
add commits for invoice class
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="23">
   <si>
     <t>Serial</t>
   </si>
@@ -73,25 +73,13 @@
     <t>SB</t>
   </si>
   <si>
-    <t>sk</t>
-  </si>
-  <si>
-    <t>, Date error in Arrival, Date error in Departure</t>
-  </si>
-  <si>
-    <t>, empty in Rate code</t>
-  </si>
-  <si>
-    <t>, Date error in Departure</t>
-  </si>
-  <si>
-    <t>, Date error in Arrival</t>
-  </si>
-  <si>
-    <t>, Date error in Res_date</t>
-  </si>
-  <si>
-    <t>error in rate code</t>
+    <t>TF</t>
+  </si>
+  <si>
+    <t>DD</t>
+  </si>
+  <si>
+    <t>DJ</t>
   </si>
   <si>
     <t>reservation date not valid</t>
@@ -456,7 +444,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -532,7 +520,7 @@
         <v>17</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I2">
         <v>54</v>
@@ -556,7 +544,7 @@
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -572,11 +560,8 @@
       <c r="D3">
         <v>161334</v>
       </c>
-      <c r="E3" s="2">
-        <v>45230</v>
-      </c>
-      <c r="F3" s="2">
-        <v>45235</v>
+      <c r="G3" t="s">
+        <v>17</v>
       </c>
       <c r="H3">
         <v>5</v>
@@ -603,7 +588,7 @@
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -619,14 +604,11 @@
       <c r="D4">
         <v>161336</v>
       </c>
-      <c r="E4" s="2">
-        <v>45230</v>
-      </c>
       <c r="G4" t="s">
         <v>17</v>
       </c>
       <c r="H4">
-        <v>-45230</v>
+        <v>5</v>
       </c>
       <c r="I4">
         <v>54</v>
@@ -666,14 +648,11 @@
       <c r="D5">
         <v>161459</v>
       </c>
-      <c r="F5" s="2">
-        <v>45239</v>
-      </c>
       <c r="G5" t="s">
         <v>17</v>
       </c>
       <c r="H5">
-        <v>45239</v>
+        <v>6</v>
       </c>
       <c r="I5">
         <v>54</v>
@@ -697,7 +676,7 @@
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -713,12 +692,6 @@
       <c r="D6">
         <v>161738</v>
       </c>
-      <c r="E6" s="2">
-        <v>45237</v>
-      </c>
-      <c r="F6" s="2">
-        <v>45243</v>
-      </c>
       <c r="G6" t="s">
         <v>17</v>
       </c>
@@ -741,10 +714,10 @@
         <v>8767.894736842105</v>
       </c>
       <c r="O6">
-        <v>1</v>
-      </c>
-      <c r="Q6">
-        <v>340.2</v>
+        <v>0</v>
+      </c>
+      <c r="P6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -760,12 +733,6 @@
       <c r="D7">
         <v>161753</v>
       </c>
-      <c r="E7" s="2">
-        <v>45237</v>
-      </c>
-      <c r="F7" s="2">
-        <v>45244</v>
-      </c>
       <c r="G7" t="s">
         <v>17</v>
       </c>
@@ -791,28 +758,25 @@
         <v>10229.21052631579</v>
       </c>
       <c r="O7">
-        <v>1</v>
-      </c>
-      <c r="Q7">
-        <v>388.8</v>
+        <v>0</v>
+      </c>
+      <c r="P7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" s="2">
+        <v>45229</v>
+      </c>
       <c r="C8">
         <v>115363600331</v>
       </c>
       <c r="D8">
         <v>161799</v>
       </c>
-      <c r="E8" s="2">
-        <v>45238</v>
-      </c>
-      <c r="F8" s="2">
-        <v>45245</v>
-      </c>
       <c r="G8" t="s">
         <v>18</v>
       </c>
@@ -841,7 +805,7 @@
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -849,49 +813,40 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>45229</v>
+        <v>45237</v>
       </c>
       <c r="C9">
-        <v>116383606590</v>
+        <v>116383610193</v>
       </c>
       <c r="D9">
-        <v>161753</v>
-      </c>
-      <c r="E9" s="2">
-        <v>45237</v>
-      </c>
-      <c r="F9" s="2">
-        <v>45244</v>
+        <v>161910</v>
       </c>
       <c r="G9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="I9">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="J9">
-        <v>378</v>
+        <v>350</v>
       </c>
       <c r="K9">
         <v>30.85</v>
       </c>
       <c r="L9">
-        <v>11661.3</v>
+        <v>10797.5</v>
       </c>
       <c r="M9">
-        <v>1432.089473684209</v>
+        <v>1326.008771929824</v>
       </c>
       <c r="N9">
-        <v>10229.21052631579</v>
+        <v>9471.491228070176</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -899,49 +854,860 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>46325</v>
+        <v>45231</v>
       </c>
       <c r="C10">
-        <v>115363600331</v>
+        <v>116353608470</v>
       </c>
       <c r="D10">
-        <v>161799</v>
-      </c>
-      <c r="E10" s="2">
+        <v>161911</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10">
+        <v>54</v>
+      </c>
+      <c r="J10">
+        <v>378</v>
+      </c>
+      <c r="K10">
+        <v>30.85</v>
+      </c>
+      <c r="L10">
+        <v>11661.3</v>
+      </c>
+      <c r="M10">
+        <v>1432.089473684209</v>
+      </c>
+      <c r="N10">
+        <v>10229.21052631579</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>45234</v>
+      </c>
+      <c r="C11">
+        <v>115363600416</v>
+      </c>
+      <c r="D11">
+        <v>161913</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11">
+        <v>50</v>
+      </c>
+      <c r="J11">
+        <v>350</v>
+      </c>
+      <c r="K11">
+        <v>30.85</v>
+      </c>
+      <c r="L11">
+        <v>10797.5</v>
+      </c>
+      <c r="M11">
+        <v>1326.008771929824</v>
+      </c>
+      <c r="N11">
+        <v>9471.491228070176</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>45234</v>
+      </c>
+      <c r="C12">
+        <v>115363600416</v>
+      </c>
+      <c r="D12">
+        <v>161914</v>
+      </c>
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12">
+        <v>50</v>
+      </c>
+      <c r="J12">
+        <v>350</v>
+      </c>
+      <c r="K12">
+        <v>30.85</v>
+      </c>
+      <c r="L12">
+        <v>10797.5</v>
+      </c>
+      <c r="M12">
+        <v>1326.008771929824</v>
+      </c>
+      <c r="N12">
+        <v>9471.491228070176</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>45231</v>
+      </c>
+      <c r="C13">
+        <v>116383608640</v>
+      </c>
+      <c r="D13">
+        <v>161916</v>
+      </c>
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13">
+        <v>54</v>
+      </c>
+      <c r="J13">
+        <v>378</v>
+      </c>
+      <c r="K13">
+        <v>30.85</v>
+      </c>
+      <c r="L13">
+        <v>11661.3</v>
+      </c>
+      <c r="M13">
+        <v>1432.089473684209</v>
+      </c>
+      <c r="N13">
+        <v>10229.21052631579</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>45236</v>
+      </c>
+      <c r="C14">
+        <v>116323611002</v>
+      </c>
+      <c r="D14">
+        <v>161980</v>
+      </c>
+      <c r="G14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14">
+        <v>129</v>
+      </c>
+      <c r="J14">
+        <v>903</v>
+      </c>
+      <c r="K14">
+        <v>30.85</v>
+      </c>
+      <c r="L14">
+        <v>27857.55</v>
+      </c>
+      <c r="M14">
+        <v>3421.102631578946</v>
+      </c>
+      <c r="N14">
+        <v>24436.44736842106</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>45234</v>
+      </c>
+      <c r="C15">
+        <v>116383609128</v>
+      </c>
+      <c r="D15">
+        <v>162029</v>
+      </c>
+      <c r="G15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15">
+        <v>50</v>
+      </c>
+      <c r="J15">
+        <v>350</v>
+      </c>
+      <c r="K15">
+        <v>30.85</v>
+      </c>
+      <c r="L15">
+        <v>10797.5</v>
+      </c>
+      <c r="M15">
+        <v>1326.008771929824</v>
+      </c>
+      <c r="N15">
+        <v>9471.491228070176</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>45232</v>
+      </c>
+      <c r="C16">
+        <v>116383608138</v>
+      </c>
+      <c r="D16">
+        <v>162033</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16">
+        <v>43</v>
+      </c>
+      <c r="J16">
+        <v>301</v>
+      </c>
+      <c r="K16">
+        <v>30.85</v>
+      </c>
+      <c r="L16">
+        <v>9285.85</v>
+      </c>
+      <c r="M16">
+        <v>1140.367543859648</v>
+      </c>
+      <c r="N16">
+        <v>8145.482456140352</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>45233</v>
+      </c>
+      <c r="C17">
+        <v>116323609306</v>
+      </c>
+      <c r="D17">
+        <v>162077</v>
+      </c>
+      <c r="G17" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17">
+        <v>54</v>
+      </c>
+      <c r="J17">
+        <v>378</v>
+      </c>
+      <c r="K17">
+        <v>30.85</v>
+      </c>
+      <c r="L17">
+        <v>11661.3</v>
+      </c>
+      <c r="M17">
+        <v>1432.089473684209</v>
+      </c>
+      <c r="N17">
+        <v>10229.21052631579</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
         <v>45238</v>
       </c>
-      <c r="F10" s="2">
-        <v>45245</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="C18">
+        <v>116373610741</v>
+      </c>
+      <c r="D18">
+        <v>162079</v>
+      </c>
+      <c r="G18" t="s">
         <v>18</v>
       </c>
-      <c r="H10">
-        <v>7</v>
-      </c>
-      <c r="I10">
+      <c r="I18">
+        <v>40</v>
+      </c>
+      <c r="J18">
+        <v>280</v>
+      </c>
+      <c r="K18">
+        <v>30.85</v>
+      </c>
+      <c r="L18">
+        <v>8638</v>
+      </c>
+      <c r="M18">
+        <v>1060.807017543859</v>
+      </c>
+      <c r="N18">
+        <v>7577.192982456141</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>45231</v>
+      </c>
+      <c r="C19">
+        <v>116323608224</v>
+      </c>
+      <c r="D19">
+        <v>162080</v>
+      </c>
+      <c r="G19" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19">
         <v>43</v>
       </c>
-      <c r="J10">
+      <c r="J19">
         <v>301</v>
       </c>
-      <c r="K10">
-        <v>30.85</v>
-      </c>
-      <c r="L10">
+      <c r="K19">
+        <v>30.85</v>
+      </c>
+      <c r="L19">
         <v>9285.85</v>
       </c>
-      <c r="M10">
+      <c r="M19">
         <v>1140.367543859648</v>
       </c>
-      <c r="N10">
+      <c r="N19">
         <v>8145.482456140352</v>
       </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10" t="s">
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>45237</v>
+      </c>
+      <c r="C20">
+        <v>116353610541</v>
+      </c>
+      <c r="D20">
+        <v>162132</v>
+      </c>
+      <c r="G20" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20">
+        <v>40</v>
+      </c>
+      <c r="J20">
+        <v>240</v>
+      </c>
+      <c r="K20">
+        <v>30.85</v>
+      </c>
+      <c r="L20">
+        <v>7404</v>
+      </c>
+      <c r="M20">
+        <v>909.2631578947367</v>
+      </c>
+      <c r="N20">
+        <v>6494.736842105263</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>45230</v>
+      </c>
+      <c r="C21">
+        <v>116373607505</v>
+      </c>
+      <c r="D21">
+        <v>162154</v>
+      </c>
+      <c r="G21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21">
+        <v>54</v>
+      </c>
+      <c r="J21">
+        <v>378</v>
+      </c>
+      <c r="K21">
+        <v>30.85</v>
+      </c>
+      <c r="L21">
+        <v>11661.3</v>
+      </c>
+      <c r="M21">
+        <v>1432.089473684209</v>
+      </c>
+      <c r="N21">
+        <v>10229.21052631579</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>45237</v>
+      </c>
+      <c r="C22">
+        <v>116373611410</v>
+      </c>
+      <c r="D22">
+        <v>162159</v>
+      </c>
+      <c r="G22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22">
+        <v>50</v>
+      </c>
+      <c r="J22">
+        <v>350</v>
+      </c>
+      <c r="K22">
+        <v>30.85</v>
+      </c>
+      <c r="L22">
+        <v>10797.5</v>
+      </c>
+      <c r="M22">
+        <v>1326.008771929824</v>
+      </c>
+      <c r="N22">
+        <v>9471.491228070176</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>45237</v>
+      </c>
+      <c r="C23">
+        <v>116373611410</v>
+      </c>
+      <c r="D23">
+        <v>162165</v>
+      </c>
+      <c r="G23" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23">
+        <v>50</v>
+      </c>
+      <c r="J23">
+        <v>350</v>
+      </c>
+      <c r="K23">
+        <v>30.85</v>
+      </c>
+      <c r="L23">
+        <v>10797.5</v>
+      </c>
+      <c r="M23">
+        <v>1326.008771929824</v>
+      </c>
+      <c r="N23">
+        <v>9471.491228070176</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>45233</v>
+      </c>
+      <c r="C24">
+        <v>116323610067</v>
+      </c>
+      <c r="D24">
+        <v>162175</v>
+      </c>
+      <c r="G24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I24">
+        <v>43</v>
+      </c>
+      <c r="J24">
+        <v>301</v>
+      </c>
+      <c r="K24">
+        <v>30.85</v>
+      </c>
+      <c r="L24">
+        <v>9285.85</v>
+      </c>
+      <c r="M24">
+        <v>1140.367543859648</v>
+      </c>
+      <c r="N24">
+        <v>8145.482456140352</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>45234</v>
+      </c>
+      <c r="C25">
+        <v>116363608907</v>
+      </c>
+      <c r="D25">
+        <v>162176</v>
+      </c>
+      <c r="G25" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25">
+        <v>54</v>
+      </c>
+      <c r="J25">
+        <v>378</v>
+      </c>
+      <c r="K25">
+        <v>30.85</v>
+      </c>
+      <c r="L25">
+        <v>11661.3</v>
+      </c>
+      <c r="M25">
+        <v>1432.089473684209</v>
+      </c>
+      <c r="N25">
+        <v>10229.21052631579</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>45237</v>
+      </c>
+      <c r="C26">
+        <v>116353610398</v>
+      </c>
+      <c r="D26">
+        <v>162177</v>
+      </c>
+      <c r="G26" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26">
+        <v>50</v>
+      </c>
+      <c r="J26">
+        <v>400</v>
+      </c>
+      <c r="K26">
+        <v>30.85</v>
+      </c>
+      <c r="L26">
+        <v>12340</v>
+      </c>
+      <c r="M26">
+        <v>1515.438596491227</v>
+      </c>
+      <c r="N26">
+        <v>10824.56140350877</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27">
         <v>26</v>
+      </c>
+      <c r="B27" s="2">
+        <v>45238</v>
+      </c>
+      <c r="C27">
+        <v>116363611495</v>
+      </c>
+      <c r="D27">
+        <v>162182</v>
+      </c>
+      <c r="G27" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27">
+        <v>50</v>
+      </c>
+      <c r="J27">
+        <v>350</v>
+      </c>
+      <c r="K27">
+        <v>30.85</v>
+      </c>
+      <c r="L27">
+        <v>10797.5</v>
+      </c>
+      <c r="M27">
+        <v>1326.008771929824</v>
+      </c>
+      <c r="N27">
+        <v>9471.491228070176</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2">
+        <v>45234</v>
+      </c>
+      <c r="C28">
+        <v>116383610612</v>
+      </c>
+      <c r="D28">
+        <v>162183</v>
+      </c>
+      <c r="G28" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28">
+        <v>54</v>
+      </c>
+      <c r="J28">
+        <v>324</v>
+      </c>
+      <c r="K28">
+        <v>30.85</v>
+      </c>
+      <c r="L28">
+        <v>9995.4</v>
+      </c>
+      <c r="M28">
+        <v>1227.505263157895</v>
+      </c>
+      <c r="N28">
+        <v>8767.894736842105</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>45232</v>
+      </c>
+      <c r="C29">
+        <v>116363609218</v>
+      </c>
+      <c r="D29">
+        <v>162197</v>
+      </c>
+      <c r="G29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I29">
+        <v>66</v>
+      </c>
+      <c r="J29">
+        <v>660</v>
+      </c>
+      <c r="K29">
+        <v>30.85</v>
+      </c>
+      <c r="L29">
+        <v>20361</v>
+      </c>
+      <c r="M29">
+        <v>2500.473684210523</v>
+      </c>
+      <c r="N29">
+        <v>17860.52631578948</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2">
+        <v>45236</v>
+      </c>
+      <c r="C30">
+        <v>116343610274</v>
+      </c>
+      <c r="D30">
+        <v>162201</v>
+      </c>
+      <c r="G30" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30">
+        <v>54</v>
+      </c>
+      <c r="J30">
+        <v>400</v>
+      </c>
+      <c r="K30">
+        <v>30.85</v>
+      </c>
+      <c r="L30">
+        <v>13327.2</v>
+      </c>
+      <c r="M30">
+        <v>1636.673684210526</v>
+      </c>
+      <c r="N30">
+        <v>11690.52631578948</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>